<commit_message>
Added information for Region header.
</commit_message>
<xml_diff>
--- a/smartgrid/dbdata/dblayout.xlsx
+++ b/smartgrid/dbdata/dblayout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Course Number</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>North, South, etc.</t>
   </si>
 </sst>
 </file>
@@ -408,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,9 +430,10 @@
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,8 +455,11 @@
       <c r="G1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -466,7 +479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -486,7 +499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -508,8 +521,11 @@
       <c r="G4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -522,28 +538,31 @@
       <c r="D5">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>

</xml_diff>